<commit_message>
Desarrollo de proceso 100
</commit_message>
<xml_diff>
--- a/Data/Output/output_datos_buscar.xlsx
+++ b/Data/Output/output_datos_buscar.xlsx
@@ -35,7 +35,7 @@
     <x:t>https://www.amazon.com/Unidapt-Adapter-Grounded-Adaptor-Converter/dp/B08D741PV6/?_encoding=UTF8&amp;pd_rd_w=jijKL&amp;content-id=amzn1.sym.59e06f17-139e-49a4-ada7-b8439f50bb02&amp;pf_rd_p=59e06f17-139e-49a4-ada7-b8439f50bb02&amp;pf_rd_r=2C0A240NGGT8EAAY6T8W&amp;pd_rd_wg=9bQhE&amp;pd_rd_r=2c145a53-a3ce-40e4-9153-dd68bc9aa91d&amp;ref_=pd_gw_exports_top_sellers_unrec&amp;language=es_US&amp;currency=CLP</x:t>
   </x:si>
   <x:si>
-    <x:t>7440</x:t>
+    <x:t>7471</x:t>
   </x:si>
   <x:si>
     <x:t>SI</x:t>
@@ -47,7 +47,7 @@
     <x:t>https://www.amazon.com/-/es/SAMSUNG-adaptador-microSDXC-MB-ME256KA-AM/dp/B09B1GXM16/?_encoding=UTF8&amp;pd_rd_w=AwyqZ&amp;content-id=amzn1.sym.10f16e90-d621-4a53-9c61-544e5c741acc&amp;pf_rd_p=10f16e90-d621-4a53-9c61-544e5c741acc&amp;pf_rd_r=2EKX99B49VGGRQT8FTMG&amp;pd_rd_wg=Ubz32&amp;pd_rd_r=33df8239-3efa-425c-a17c-d80ff98a173b&amp;ref_=pd_gw_exports_top_sellers_unrec</x:t>
   </x:si>
   <x:si>
-    <x:t>27311</x:t>
+    <x:t>27424</x:t>
   </x:si>
   <x:si>
     <x:t>KSIPZE Tira de luces LED de 100 pies</x:t>
@@ -56,7 +56,7 @@
     <x:t>https://www.amazon.com/-/es/sincronizaci%C3%B3n-aplicaci%C3%B3n-inteligente-dormitorio-iluminaci%C3%B3n/dp/B09V366BDY/ref=sr_1_5?_encoding=UTF8&amp;content-id=amzn1.sym.7738c60e-a1c7-4678-9812-5d82959d511c&amp;keywords=strip+lighting&amp;pd_rd_r=a61aa239-6f17-4b90-b50e-30ac73d896ec&amp;pd_rd_w=GCgMp&amp;pd_rd_wg=8Tbic&amp;pf_rd_p=7738c60e-a1c7-4678-9812-5d82959d511c&amp;pf_rd_r=WXPCKCN6VR02D770X6QB&amp;qid=1691511023&amp;sr=8-5</x:t>
   </x:si>
   <x:si>
-    <x:t>11164</x:t>
+    <x:t>11211</x:t>
   </x:si>
   <x:si>
     <x:t>Black &amp; Decker Horno tostador</x:t>
@@ -65,7 +65,7 @@
     <x:t>https://www.amazon.com/Black-Decker-Horno-tostador-Posiciones/dp/B0043E6PLC/ref=sr_1_2_sspa?__mk_es_US=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=294JUCGTJ8SVX&amp;keywords=oven&amp;qid=1691511097&amp;sprefix=ov%2Caps%2C210&amp;sr=8-2-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1</x:t>
   </x:si>
   <x:si>
-    <x:t>83794</x:t>
+    <x:t>84143</x:t>
   </x:si>
   <x:si>
     <x:t>NO</x:t>
@@ -77,7 +77,7 @@
     <x:t>https://www.amazon.com/-/es/Speedster-SWFT-Radeon-6600-CORE/dp/B09HHLX543/?_encoding=UTF8&amp;pd_rd_w=NQ3Jj&amp;content-id=amzn1.sym.10f16e90-d621-4a53-9c61-544e5c741acc&amp;pf_rd_p=10f16e90-d621-4a53-9c61-544e5c741acc&amp;pf_rd_r=H7T3R6A6NRXSEGA806SJ&amp;pd_rd_wg=VsEIi&amp;pd_rd_r=8e02ff95-d2c0-4b6f-a03f-3c0e37c5d72b&amp;ref_=pd_gw_exports_top_sellers_unrec</x:t>
   </x:si>
   <x:si>
-    <x:t>186221</x:t>
+    <x:t>186997</x:t>
   </x:si>
   <x:si>
     <x:t>Flopping Fish</x:t>
@@ -95,7 +95,7 @@
     <x:t>https://www.amazon.com/Masterworks-Publishing/dp/B09XDKH164/ref=sr_1_4_sspa?__mk_es_US=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=LP1VB31Z5UX5&amp;keywords=sheet+music&amp;qid=1691524986&amp;sprefix=sheet+musi%2Caps%2C205&amp;sr=8-4-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1</x:t>
   </x:si>
   <x:si>
-    <x:t>14368</x:t>
+    <x:t>14456</x:t>
   </x:si>
   <x:si>
     <x:t>Mueller 7-inch Meat Cleaver Knife</x:t>
@@ -104,7 +104,7 @@
     <x:t>https://www.amazon.com/SS-77/dp/B08BX7FMQN/ref=sxin_16_pa_sp_search_thematic_sspa?__mk_es_US=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;_encoding=UTF8&amp;content-id=amzn1.sym.1c86ab1a-a73c-4131-85f1-15bd92ae152d%3Aamzn1.sym.1c86ab1a-a73c-4131-85f1-15bd92ae152d&amp;crid=1I6JCWDEKEH2U&amp;cv_ct_cx=home+and+kitchen&amp;keywords=hogar+y+cocina&amp;pd_rd_i=B08BX7FMQN&amp;pd_rd_r=9e6d404a-6a8f-42eb-b5d8-c1690bcb9052&amp;pd_rd_w=9oCTs&amp;pd_rd_wg=1Erix&amp;pf_rd_p=1c86ab1a-a73c-4131-85f1-15bd92ae152d&amp;pf_rd_r=VD71XTE1EH7WYGT6DQ1T&amp;qid=1691525059&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sprefix=hogar%2Caps%2C278&amp;sr=1-2-364cf978-ce2a-480a-9bb0-bdb96faa0f61-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9zZWFyY2hfdGhlbWF0aWM&amp;psc=1&amp;smid=A8I6IE7ASKFON</x:t>
   </x:si>
   <x:si>
-    <x:t>14889</x:t>
+    <x:t>14951</x:t>
   </x:si>
   <x:si>
     <x:t>Utopia Towels 6 Pack Premium Hand Towels Set</x:t>
@@ -113,7 +113,7 @@
     <x:t>https://www.amazon.com/Utopia-Towels-Premium-Grey-Hand/dp/B083KKF8F8/ref=sr_1_1_sspa?crid=1KDZABCENUGOT&amp;keywords=hand%2Btowel&amp;qid=1691525294&amp;sprefix=hand%2Btowe%2Caps%2C290&amp;sr=8-1-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;th=1</x:t>
   </x:si>
   <x:si>
-    <x:t>17124</x:t>
+    <x:t>17195</x:t>
   </x:si>
   <x:si>
     <x:t>Amazon Basics Neoprene Workout Dumbbell</x:t>
@@ -128,7 +128,7 @@
     <x:t>https://www.amazon.com/Google-Pixel-7a-Unlocked-Smartphone/dp/B0BZ9T8R41/ref=sr_1_1_sspa?crid=2PWFCK2DVYVOQ&amp;keywords=nothing%2Bphone&amp;qid=1691525818&amp;sprefix=nothing%2Bpho%2Caps%2C266&amp;sr=8-1-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;th=1</x:t>
   </x:si>
   <x:si>
-    <x:t>464644</x:t>
+    <x:t>466580</x:t>
   </x:si>
   <x:si>
     <x:t>Flameless LED Tea Light Candles</x:t>
@@ -149,7 +149,7 @@
     <x:t>https://www.amazon.com/THERMOS-FUNTAINER-Ounce-Stainless-Steel/dp/B08NCVT244/?_encoding=UTF8&amp;pd_rd_w=mt2Uz&amp;content-id=amzn1.sym.59e06f17-139e-49a4-ada7-b8439f50bb02&amp;pf_rd_p=59e06f17-139e-49a4-ada7-b8439f50bb02&amp;pf_rd_r=V6B2WJ56S9ZNKER7M4XC&amp;pd_rd_wg=bW0kF&amp;pd_rd_r=39e09029-a613-414c-b146-91b724c083f6&amp;ref_=pd_gw_exports_top_sellers_unrec&amp;th=1</x:t>
   </x:si>
   <x:si>
-    <x:t>13399</x:t>
+    <x:t>13455</x:t>
   </x:si>
   <x:si>
     <x:t>Hoppy The Bunny</x:t>
@@ -158,7 +158,7 @@
     <x:t>https://www.amazon.com/Westminster-SG_B01D0JLWVS_US-Hoppy-Mechanical-Bunny/dp/B01D0JLWVS/?_encoding=UTF8&amp;pd_rd_w=nr0zp&amp;content-id=amzn1.sym.59e06f17-139e-49a4-ada7-b8439f50bb02&amp;pf_rd_p=59e06f17-139e-49a4-ada7-b8439f50bb02&amp;pf_rd_r=MDE7HD64PQJ567XNG0AN&amp;pd_rd_wg=c2YVK&amp;pd_rd_r=a11c1dd4-e1b0-4b95-8f14-c0394d94c9ad&amp;ref_=pd_gw_exports_top_sellers_unrec</x:t>
   </x:si>
   <x:si>
-    <x:t>13306</x:t>
+    <x:t>13362</x:t>
   </x:si>
   <x:si>
     <x:t>MRbrew</x:t>
@@ -167,7 +167,7 @@
     <x:t>https://www.amazon.com/MRbrew-American-System-Picnic-Chrome-Plated/dp/B07YV341NZ/ref=sr_1_5?crid=2HBGCH5YN2KYS&amp;keywords=party+pump&amp;qid=1691528197&amp;sprefix=party+pum%2Caps%2C215&amp;sr=8-5</x:t>
   </x:si>
   <x:si>
-    <x:t>39099</x:t>
+    <x:t>39262</x:t>
   </x:si>
   <x:si>
     <x:t>Pokemon - Charizard - XY Evo</x:t>
@@ -176,7 +176,7 @@
     <x:t>https://www.amazon.com/Pokemon-Charizard-108-Evolutions-Holo/dp/B01M4QJUOL/ref=sr_1_4?crid=H03KFBNOM58D&amp;keywords=charizard+card&amp;qid=1691528233&amp;sprefix=charizard+ca%2Caps%2C203&amp;sr=8-4</x:t>
   </x:si>
   <x:si>
-    <x:t>62182</x:t>
+    <x:t>71025</x:t>
   </x:si>
   <x:si>
     <x:t>Cinderace Vmax</x:t>
@@ -191,7 +191,7 @@
     <x:t>https://www.amazon.com/Officemate-26092-Letter-Recycled-Black/dp/B003G4MNUW/?_encoding=UTF8&amp;_ref=dlx_gate_sd_dcl_tlt_59c541b0_dt&amp;pd_rd_w=jLN8Q&amp;content-id=amzn1.sym.81a68cec-8afc-4296-99f7-78cf5ddc15b5&amp;pf_rd_p=81a68cec-8afc-4296-99f7-78cf5ddc15b5&amp;pf_rd_r=2QVJ5A934TS0CZGC7TJR&amp;pd_rd_wg=qJq5x&amp;pd_rd_r=91a44954-47ba-4559-9e57-788901623031&amp;ref_=pd_gw_unk</x:t>
   </x:si>
   <x:si>
-    <x:t>29517</x:t>
+    <x:t>29640</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>